<commit_message>
Refactor damage calculation documentation for clarity and consistency
</commit_message>
<xml_diff>
--- a/posts/xcxde/inner.xlsx
+++ b/posts/xcxde/inner.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
   <si>
     <t>基礎ステータス</t>
   </si>
@@ -254,6 +254,274 @@
   </si>
   <si>
     <t>サイトアップ/スナイパーライフル</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>加算ボーナス</t>
+    <rPh sb="0" eb="2">
+      <t>カサン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>名前</t>
+    <rPh sb="0" eb="2">
+      <t>ナマエ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>%</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>オーバークロックギア</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>開幕アーツ</t>
+    <rPh sb="0" eb="2">
+      <t>カイマク</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>未発見時のみ有効</t>
+    <rPh sb="0" eb="3">
+      <t>ミハッケン</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ユウコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ソウルボイス</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>バレットチャージ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ユニオンサポート</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>転倒</t>
+    <rPh sb="0" eb="2">
+      <t>テントウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>スタン</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>キャッチ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>クリティカル</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>レベル差補正</t>
+    <rPh sb="3" eb="4">
+      <t>サ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ホセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>12*(レベル差)%</t>
+    <rPh sb="7" eb="8">
+      <t>サ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>敵が攻撃側の場合のみ適用
+敵がLv60以上の場合は、Lv60とみなして計算</t>
+    <rPh sb="0" eb="1">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>コウゲキ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ガワ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>テキヨウ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ケイサン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>敵が攻撃側の場合のみ適用</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>部位破壊</t>
+    <rPh sb="0" eb="2">
+      <t>ブイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ハカイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ドールディフェンス</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>会心強化で増加</t>
+    <rPh sb="0" eb="2">
+      <t>カイシン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キョウカ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ゾウカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ほとんどのスキル</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>属性強化</t>
+    <rPh sb="0" eb="2">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キョウカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>オーラの強化</t>
+    <rPh sb="4" eb="6">
+      <t>キョウカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>条件付き強化</t>
+    <rPh sb="0" eb="3">
+      <t>ジョウケンツ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>キョウカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>備考</t>
+    <rPh sb="0" eb="2">
+      <t>ビコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>流星乱舞・ボルテージマックスなど</t>
+    <rPh sb="0" eb="2">
+      <t>リュウセイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ランブ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>インサイドブレイカー・バトルフェンサーを除く</t>
+    <rPh sb="20" eb="21">
+      <t>ノゾ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>位置特効</t>
+    <rPh sb="0" eb="2">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>トッコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>エーテル攻撃強化など</t>
+    <rPh sb="4" eb="6">
+      <t>コウゲキ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>キョウカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ビーストキラーなど</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>種族特効</t>
+    <rPh sb="0" eb="2">
+      <t>シュゾク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>トッコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>10*(破壊数)%</t>
+    <rPh sb="4" eb="6">
+      <t>ハカイ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>スウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>max +500%</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>max +300%</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ナイトスコープ</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -648,10 +916,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A2:J53"/>
+  <dimension ref="A2:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -667,7 +935,7 @@
     <col min="11" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -823,7 +1091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1089,7 +1357,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
@@ -1118,7 +1386,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1205,102 +1473,280 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="27" x14ac:dyDescent="0.15">
-      <c r="A42" s="6" t="s">
+    <row r="26" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+      <c r="B27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+      <c r="B30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="B33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B35" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="B36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B37" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="B38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B41" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B42" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="B44" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" s="1">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="B45" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="A52" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B43" s="3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B53" s="3">
         <v>5</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C53" s="4">
         <v>-0.85</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B44" s="3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B54" s="3">
         <v>4</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C54" s="4">
         <v>-0.75</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B45" s="3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B55" s="3">
         <v>3</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C55" s="4">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B46" s="3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B56" s="3">
         <v>2</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C56" s="4">
         <v>-0.25</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B47" s="3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B57" s="3">
         <v>1</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C57" s="4">
         <v>-0.15</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B48" s="2" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B58" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B49" s="3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B59" s="3">
         <v>-1</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C59" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B50" s="3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B60" s="3">
         <v>-2</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C60" s="4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B51" s="3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B61" s="3">
         <v>-3</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C61" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B52" s="3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B62" s="3">
         <v>-4</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C62" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B53" s="3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B63" s="3">
         <v>-5</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C63" s="4">
         <v>1.5</v>
       </c>
     </row>

</xml_diff>